<commit_message>
Agora vai hein galerinha
</commit_message>
<xml_diff>
--- a/Catarse/Orçamento.xlsx
+++ b/Catarse/Orçamento.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Domínio Hedtrot.com + SSL</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Recompensas</t>
+  </si>
+  <si>
+    <t>Livros</t>
   </si>
 </sst>
 </file>
@@ -684,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.25"/>
@@ -840,12 +843,11 @@
       <c r="A6" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="17"/>
+      <c r="B6" s="17">
+        <v>20</v>
+      </c>
       <c r="C6" s="20"/>
-      <c r="D6" s="24">
-        <f>((C6*G2)+((C6*G2)*G5))</f>
-        <v>0</v>
-      </c>
+      <c r="D6" s="24"/>
       <c r="E6" s="4"/>
       <c r="F6" s="33">
         <v>0.13</v>
@@ -937,7 +939,7 @@
       <c r="F9" s="4"/>
       <c r="G9" s="41">
         <f>(D14*0.13)</f>
-        <v>102.59836600000001</v>
+        <v>144.87566600000002</v>
       </c>
       <c r="H9" s="41"/>
       <c r="I9" s="2"/>
@@ -951,10 +953,16 @@
       <c r="Q9" s="2"/>
     </row>
     <row r="10" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="17"/>
+      <c r="A10" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="17">
+        <v>2</v>
+      </c>
       <c r="C10" s="20"/>
-      <c r="D10" s="24"/>
+      <c r="D10" s="24">
+        <v>325.20999999999998</v>
+      </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -1021,7 +1029,7 @@
       <c r="F13" s="4"/>
       <c r="G13" s="41">
         <f>D14+G9</f>
-        <v>891.81656600000008</v>
+        <v>1259.3038660000002</v>
       </c>
       <c r="H13" s="41"/>
       <c r="I13" s="2"/>
@@ -1045,7 +1053,7 @@
       </c>
       <c r="D14" s="24">
         <f>SUM(D2:D12)</f>
-        <v>789.21820000000002</v>
+        <v>1114.4282000000001</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>

</xml_diff>